<commit_message>
Added more learning content and questions to the easy level
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="74">
   <si>
     <t>question</t>
   </si>
@@ -35,19 +35,7 @@
     <t>hint2</t>
   </si>
   <si>
-    <t>This is an introduction to probability</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>Through this game you will learn probability concepts such as Bays rule, and conditional probability</t>
-  </si>
-  <si>
-    <t>A set is a collection of distinct obejcts</t>
-  </si>
-  <si>
-    <t>If you have 2 sets, A and B, and set B fully encompasses set A, then set A is considered to be a subset of B</t>
   </si>
   <si>
     <t>A ⊆ B</t>
@@ -170,12 +158,153 @@
   <si>
     <t>P(N)</t>
   </si>
+  <si>
+    <t>If you have 2 sets, A and B, and set B fully encompasses set A, then set A is considered to be a subset of B.</t>
+  </si>
+  <si>
+    <t>How many squares make up the neuron? How many squares make up the electrode array?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock or dendrite? </t>
+  </si>
+  <si>
+    <t>P(AH) + P(D)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you choose a square at random from the electrode array, what is the probability of choosing the axon or dendrite? </t>
+  </si>
+  <si>
+    <t>P(A) + P(D)</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock?</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of choosing any part of the axon?</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of choosing any part of the dendrite?</t>
+  </si>
+  <si>
+    <t>P(A)</t>
+  </si>
+  <si>
+    <t>P(D)</t>
+  </si>
+  <si>
+    <t>Welcome to USS Sampson's Neuron Battleship!</t>
+  </si>
+  <si>
+    <t>We will take you through an introduction of probability and learn concepts such as Bayes rule and conditional probability</t>
+  </si>
+  <si>
+    <t>Here you will see how to play and interact with the game. Go ahead, press the enter key.</t>
+  </si>
+  <si>
+    <t>Press the enter key on your keyboard.</t>
+  </si>
+  <si>
+    <t>I am hint 1.</t>
+  </si>
+  <si>
+    <t>I am hint 2. Now press the enter key.</t>
+  </si>
+  <si>
+    <t>Great! You are already a pro. Now the game will have three levels.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You have been assigned to take on the mission of location where our battleship is. </t>
+  </si>
+  <si>
+    <t>We will first start with the basics of Set Theory. A set is a collection of distinct events or obejcts.</t>
+  </si>
+  <si>
+    <t>Example: coin flip. S={H,T}.</t>
+  </si>
+  <si>
+    <t>Example: dice roll. S={1,2,3,4,5,6}.</t>
+  </si>
+  <si>
+    <t>What is the probability of choosing a random square or electrode from the electrode array?</t>
+  </si>
+  <si>
+    <t>P(E)</t>
+  </si>
+  <si>
+    <t>How many electrodes are in the electrode array?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Law of total probability </t>
+  </si>
+  <si>
+    <t>If A and B are mutually exclusive, P(A∩B)=0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(A)≤1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you have a set S containing an event w, we would write w∈S. (And if it’s not in S, we write w∉S.) </t>
+  </si>
+  <si>
+    <t>Here we have an electrode array or a set EA. It is composed of 64 electrodes or objects e. So e∈EA.</t>
+  </si>
+  <si>
+    <t>P(A∪B)=P(A)+P(B)-P(A∩B)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awesome job so far. Now lets learn about independence. Two events are independent if and only if P(A∩B) = P(A) P(B). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(Ac)=1-P(A), where Ac is the complement of A </t>
+  </si>
+  <si>
+    <t>P(B)=P(B∩A)+P(B∩Ac).</t>
+  </si>
+  <si>
+    <t>Good job! You got your first question right. We will find our battleship in no time. Now lets learn about our neuron.</t>
+  </si>
+  <si>
+    <t>As you can see our neuron is composed of dendrites (D), axons (A), and a axon hillock (AH).</t>
+  </si>
+  <si>
+    <t>through each level. So lets begin!</t>
+  </si>
+  <si>
+    <t>Good job! If you need any help, just press the hint button on the righ in the Notebook. Try it now.</t>
+  </si>
+  <si>
+    <t>Awesome! We will have our battleship in no time. Lets further learn about sets.</t>
+  </si>
+  <si>
+    <t>If you two sets, A and B, then their intersection denoted as A∩B. This means all the outcomes are only in both A and B.</t>
+  </si>
+  <si>
+    <t>Example: Roll of a dice.  Let A be the event that the result is &gt; 3, and B be the event that the result is even. Then A∩B={4,6}.</t>
+  </si>
+  <si>
+    <t>And if the two events have an empty intersection, then they are mutually exclusive or disjoint.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example: A be the event that roll is odd and B be the event that the roll is even. Here A and B are disjoint. </t>
+  </si>
+  <si>
+    <t>Is P(D) and P(AH) mustually exclusive?</t>
+  </si>
+  <si>
+    <t>Concepts to implement still:</t>
+  </si>
+  <si>
+    <t>If you two sets, A and B, then their union is denoted as A∪B. This means all the outcomes are in either A or B or in both A and B.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example: Roll of a dice. Let A be the event that the result is &gt; 3, and B be the event that the result is even. Then A∪B = {2,4,5,6}. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -201,25 +330,6 @@
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF252525"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -261,6 +371,17 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF252525"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -300,7 +421,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -318,37 +439,154 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -357,6 +595,62 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -365,6 +659,62 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -694,210 +1044,382 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="93.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="117.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="39.33203125" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1"/>
-    <row r="3" spans="1:5" ht="15" thickBot="1">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45">
+      <c r="A19" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="9"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="15" thickBot="1">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1">
-      <c r="A6" s="2" t="s">
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1"/>
-    <row r="11" spans="1:5" ht="15" thickBot="1">
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" thickBot="1">
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1">
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" thickBot="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" thickBot="1">
-      <c r="A19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" thickBot="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" thickBot="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" thickBot="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" thickBot="1">
-      <c r="A24" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" thickBot="1">
-      <c r="A25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5" ht="15" thickBot="1">
-      <c r="A26" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="D43" s="9"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="8"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="D46" s="9"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="D48" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -938,24 +1460,24 @@
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
-        <v>18</v>
+      <c r="A3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="6" t="s">
-        <v>20</v>
+      <c r="A4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
-        <v>17</v>
+      <c r="A5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -970,60 +1492,75 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A10" sqref="A10:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="111.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="7"/>
+    <col min="1" max="1" width="111.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1"/>
     <row r="4" spans="1:4" ht="31" thickBot="1">
-      <c r="A4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>5</v>
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="31" thickBot="1">
-      <c r="A5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>5</v>
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="31" thickBot="1">
-      <c r="A6" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>5</v>
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="10" t="s">
-        <v>29</v>
+      <c r="A8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the wording in Questions.xlsx
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="3820" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="3380" yWindow="780" windowWidth="25600" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
@@ -122,130 +122,139 @@
     <t>@n</t>
   </si>
   <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing any part of the neuron?</t>
-  </si>
-  <si>
     <t>P(N)</t>
   </si>
   <si>
     <t>How many squares make up the neuron? How many squares make up the electrode array?</t>
   </si>
   <si>
+    <t>P(AH)</t>
+  </si>
+  <si>
+    <t>P(A)</t>
+  </si>
+  <si>
+    <t>P(D)</t>
+  </si>
+  <si>
+    <t>@KeyPressed</t>
+  </si>
+  <si>
+    <t>If you two sets, A and B, then their union is denoted as A∪B. This means all the outcomes are in either A or B or in both A and B.</t>
+  </si>
+  <si>
+    <t>@KeyPressed</t>
+  </si>
+  <si>
+    <t>Example: Roll of a dice. Let A be the event that the result is &gt; 3, and B be the event that the result is even. Then A∪B = {2,4,5,6}.</t>
+  </si>
+  <si>
+    <t>If you two sets, A and B, then their intersection denoted as A∩B. This means all the outcomes are only in both A and B.</t>
+  </si>
+  <si>
+    <t>@KeyPressed</t>
+  </si>
+  <si>
+    <t>Example: Roll of a dice.  Let A be the event that the result is &gt; 3, and B be the event that the result is even. Then A∩B={4,6}.</t>
+  </si>
+  <si>
+    <t>And if the two events have an empty intersection, then they are mutually exclusive or disjoint.</t>
+  </si>
+  <si>
+    <t>@KeyPressed</t>
+  </si>
+  <si>
+    <t>Example: A be the event that roll is odd and B be the event that the roll is even. Here A and B are disjoint.</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock or axon?</t>
+  </si>
+  <si>
+    <t>P(AH) + P(A)</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock or dendrite?</t>
+  </si>
+  <si>
+    <t>P(AH) + P(D)</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon or dendrite?</t>
+  </si>
+  <si>
+    <t>P(A) + P(D)</t>
+  </si>
+  <si>
+    <t>Awesome job so far. Now lets learn about independence. Two events are independent if and only if P(A∩B) = P(A) P(B).</t>
+  </si>
+  <si>
+    <t>@KeyPressed</t>
+  </si>
+  <si>
+    <t>Is the probability of choosing a dendrite square independent of the probability of choosing an axon square?</t>
+  </si>
+  <si>
+    <t>P(A) ⊥ P(D)</t>
+  </si>
+  <si>
+    <t>Concepts to implement still:</t>
+  </si>
+  <si>
+    <t>If you have 2 sets, A and B, and set B fully encompasses set A, then set A is considered to be a subset of B.</t>
+  </si>
+  <si>
+    <t>@KeyPressed</t>
+  </si>
+  <si>
+    <t>A ⊆ B</t>
+  </si>
+  <si>
+    <t>P(A)≤1</t>
+  </si>
+  <si>
+    <t>A ∪ B = B ∪ A.</t>
+  </si>
+  <si>
+    <t>P(Ac)=1-P(A), where Ac is the complement of A</t>
+  </si>
+  <si>
+    <t>If A and B are mutually exclusive, P(A∩B)=0</t>
+  </si>
+  <si>
+    <t>P(A∪B)=P(A)+P(B)-P(A∩B)</t>
+  </si>
+  <si>
+    <t>Law of total probability</t>
+  </si>
+  <si>
+    <t>P(B)=P(B∩A)+P(B∩Ac).</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>hint1</t>
+  </si>
+  <si>
+    <t>hint2</t>
+  </si>
+  <si>
     <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock?</t>
   </si>
   <si>
     <t>P(AH)</t>
   </si>
   <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing any part of the axon?</t>
-  </si>
-  <si>
-    <t>P(A)</t>
-  </si>
-  <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing any part of the dendrite?</t>
-  </si>
-  <si>
-    <t>P(D)</t>
-  </si>
-  <si>
-    <t>Awesome! We will have our battleship in no time. Lets further learn about sets.</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>If you two sets, A and B, then their union is denoted as A∪B. This means all the outcomes are in either A or B or in both A and B.</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>Example: Roll of a dice. Let A be the event that the result is &gt; 3, and B be the event that the result is even. Then A∪B = {2,4,5,6}.</t>
-  </si>
-  <si>
-    <t>If you two sets, A and B, then their intersection denoted as A∩B. This means all the outcomes are only in both A and B.</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>Example: Roll of a dice.  Let A be the event that the result is &gt; 3, and B be the event that the result is even. Then A∩B={4,6}.</t>
-  </si>
-  <si>
-    <t>And if the two events have an empty intersection, then they are mutually exclusive or disjoint.</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>Example: A be the event that roll is odd and B be the event that the roll is even. Here A and B are disjoint.</t>
-  </si>
-  <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock or axon?</t>
-  </si>
-  <si>
-    <t>P(AH) + P(A)</t>
-  </si>
-  <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock or dendrite?</t>
-  </si>
-  <si>
-    <t>P(AH) + P(D)</t>
-  </si>
-  <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon or dendrite?</t>
-  </si>
-  <si>
-    <t>P(A) + P(D)</t>
-  </si>
-  <si>
-    <t>Is P(D) and P(AH) mustually exclusive?</t>
-  </si>
-  <si>
-    <t>Awesome job so far. Now lets learn about independence. Two events are independent if and only if P(A∩B) = P(A) P(B).</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>Is the probability of choosing a dendrite square independent of the probability of choosing an axon square?</t>
-  </si>
-  <si>
-    <t>P(A) ⊥ P(D)</t>
-  </si>
-  <si>
-    <t>Concepts to implement still:</t>
-  </si>
-  <si>
-    <t>If you have 2 sets, A and B, and set B fully encompasses set A, then set A is considered to be a subset of B.</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>A ⊆ B</t>
-  </si>
-  <si>
-    <t>P(A)≤1</t>
-  </si>
-  <si>
-    <t>A ∪ B = B ∪ A.</t>
-  </si>
-  <si>
-    <t>P(Ac)=1-P(A), where Ac is the complement of A</t>
-  </si>
-  <si>
-    <t>If A and B are mutually exclusive, P(A∩B)=0</t>
-  </si>
-  <si>
-    <t>P(A∪B)=P(A)+P(B)-P(A∩B)</t>
-  </si>
-  <si>
-    <t>Law of total probability</t>
-  </si>
-  <si>
-    <t>P(B)=P(B∩A)+P(B∩Ac).</t>
+    <t>Given that the square you chose is part of the neuron, what is the probability you chose the axon hillock?</t>
+  </si>
+  <si>
+    <t>P(AH|N)</t>
+  </si>
+  <si>
+    <t>Given no part of the neuron exists behind grey squares, what is the probability of finding the axon hillock behind each green square?</t>
   </si>
   <si>
     <t>question</t>
@@ -260,33 +269,6 @@
     <t>hint2</t>
   </si>
   <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon hillock?</t>
-  </si>
-  <si>
-    <t>P(AH)</t>
-  </si>
-  <si>
-    <t>Given that the square you chose is part of the neuron, what is the probability you chose the axon hillock?</t>
-  </si>
-  <si>
-    <t>P(AH|N)</t>
-  </si>
-  <si>
-    <t>Given no part of the neuron exists behind grey squares, what is the probability of finding the axon hillock behind each green square?</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>answer</t>
-  </si>
-  <si>
-    <t>hint1</t>
-  </si>
-  <si>
-    <t>hint2</t>
-  </si>
-  <si>
     <t>Game Play The player is given a board and the neuron they must find. For each place (square) they guess,</t>
   </si>
   <si>
@@ -330,6 +312,24 @@
   </si>
   <si>
     <t>such as Bayes rule and conditional probability through each level. So lets begin!</t>
+  </si>
+  <si>
+    <t>Awesome! We will find our battleship in no time. Lets further learn about sets.</t>
+  </si>
+  <si>
+    <t>Are P(D) and P(AH) mutually exclusive?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you choose a square at random from the electrode array, what is the probability of hitting any part of the neuron? </t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of hitting the axon hillock?</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of hitting any part of the axon?</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of hitting any part of the dendrite?</t>
   </si>
 </sst>
 </file>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -830,7 +830,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -848,7 +848,7 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -862,7 +862,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -890,7 +890,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>13</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>14</v>
@@ -1014,25 +1014,25 @@
     </row>
     <row r="19" spans="1:6" ht="45" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1040,11 +1040,11 @@
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="1"/>
@@ -1052,11 +1052,11 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="1"/>
@@ -1072,10 +1072,10 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1084,13 +1084,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1112,13 +1112,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1126,11 +1126,11 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1138,11 +1138,11 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1150,11 +1150,11 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="3"/>
@@ -1162,7 +1162,7 @@
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1180,10 +1180,10 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="1"/>
@@ -1192,11 +1192,11 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="3"/>
@@ -1212,7 +1212,7 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1222,13 +1222,13 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="3"/>
@@ -1236,11 +1236,11 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="3"/>
@@ -1248,7 +1248,7 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1258,7 +1258,7 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1268,7 +1268,7 @@
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1278,11 +1278,11 @@
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="5" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="1"/>
@@ -1344,16 +1344,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
@@ -1361,23 +1361,23 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
@@ -1449,16 +1449,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -1481,10 +1481,10 @@
     </row>
     <row r="4" spans="1:6" ht="30.75" customHeight="1">
       <c r="A4" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -1505,10 +1505,10 @@
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -1543,7 +1543,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -1553,7 +1553,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>

</xml_diff>

<commit_message>
editting excel and question
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="126">
   <si>
     <t>question</t>
   </si>
@@ -100,18 +100,12 @@
     <t>@KeyPressed</t>
   </si>
   <si>
-    <t>What is the probability of choosing a random square or electrode from the electrode array?</t>
-  </si>
-  <si>
     <t>P(E)</t>
   </si>
   <si>
     <t>How many electrodes are in the electrode array?</t>
   </si>
   <si>
-    <t>Good job! You got your first question right. We will find our battleship in no time. Now lets learn about our neuron.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
@@ -196,15 +190,6 @@
     <t>P(AH)</t>
   </si>
   <si>
-    <t>Given that the square you chose is part of the neuron, what is the probability you chose the axon hillock?</t>
-  </si>
-  <si>
-    <t>P(AH|N)</t>
-  </si>
-  <si>
-    <t>Given no part of the neuron exists behind grey squares, what is the probability of finding the axon hillock behind each green square?</t>
-  </si>
-  <si>
     <t>question</t>
   </si>
   <si>
@@ -217,42 +202,24 @@
     <t>hint2</t>
   </si>
   <si>
-    <t>Game Play The player is given a board and the neuron they must find. For each place (square) they guess,</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
-    <t>they determine the probability that the neuron is there, updating their estimates using prior information from their previous guesses</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
-    <t>. Once they find part of the neuron their final task is to find the axon hillock.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
-    <t>Given no part of the neuron exists behind grey squares, what is the probability of finding part of the neuron behind each green square?</t>
-  </si>
-  <si>
     <t>Where do you guess the neuron might be?</t>
   </si>
   <si>
     <t>What is the probability that any part of the neuron is there?</t>
   </si>
   <si>
-    <t>What is the probability that the axon hillock is there?</t>
-  </si>
-  <si>
     <t>.</t>
   </si>
   <si>
-    <t>If you choose a square at random from the neuron, what is the probability of choosing the axon?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @probAxnNrn</t>
   </si>
   <si>
@@ -313,9 +280,6 @@
     <t>The neuron is modelled in color at the top right corner of this figure.</t>
   </si>
   <si>
-    <t>How many colored squares make up the neuron shown in the upper left hand corner?</t>
-  </si>
-  <si>
     <t>If you have two sets, A and B, then their union is denoted as AuB. This means all the outcomes are in either A or B or in both A and B.</t>
   </si>
   <si>
@@ -325,9 +289,6 @@
     <t>Example: Roll of a dice.  Let A be the event that the result is &gt; 3, and B be the event that the result is even. Then AnB={4,6}.</t>
   </si>
   <si>
-    <t>Awesome job so far. Now lets learn about independence. Independence means there is thte occurance of one event has no bearing on the possibility of occurance for the other. Numerically, two events are independent if and only if P(AnB) = P(A) P(B).</t>
-  </si>
-  <si>
     <t>Are P(D) and P(AH) mutually exclusive? (y/n)</t>
   </si>
   <si>
@@ -346,10 +307,103 @@
     <t>P(B)=P(BnA)+P(BnAc).</t>
   </si>
   <si>
-    <t>Behind which of the electrodes can the axon hillock exist? Click the squares, correct guesses will change color.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @findAxnHil</t>
+  </si>
+  <si>
+    <t>When choosing an electrode at random form this array, what is the probability of choosing the electrode at (3,3)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Now lets learn about our neuron.</t>
+  </si>
+  <si>
+    <t>How many colored squares make up the neuron shown in the upper right hand corner?</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the neuron, what is the probability of choosing the axon hillock?</t>
+  </si>
+  <si>
+    <t>Independence means there is thte occurance of one event has no bearing on the possibility of occurance for the other. Numerically, two events are independent if and only if P(AnB) = P(A) P(B).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Awesome job so far. Now lets learn about independence. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game Play The player is given a board and the neuron they must find. </t>
+  </si>
+  <si>
+    <t>the player must click a location on the board and then calculate the probability that the neuron is behind it</t>
+  </si>
+  <si>
+    <t>The board will change colors depending on if part of the neuron is behind that electrode or not</t>
+  </si>
+  <si>
+    <t>The player will use prior information about where the neuron is not to calculate the probability part of the neuron is there</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @hard1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @hard2</t>
+  </si>
+  <si>
+    <t>The player has 15 chances to gues a location. The game ends when they have located the entire neuron</t>
+  </si>
+  <si>
+    <t>Are you ready to play? Press continue.</t>
+  </si>
+  <si>
+    <t>There are 2 ways to calculate conditional probability</t>
+  </si>
+  <si>
+    <t>The conditional probability of A given B denoted as P(A|B) is defined as P(AnB)/P(B)</t>
+  </si>
+  <si>
+    <t>But it can also be calculated using Bayes Rule</t>
+  </si>
+  <si>
+    <t>Bayes Rule states that P(A|B) = P(B|A)*P(A)/P(B)</t>
+  </si>
+  <si>
+    <t>We will practice calculating the conditional probabilty using both methods to show their equivalence</t>
+  </si>
+  <si>
+    <t>Do you see the ___ square on the board? This color denotes that no part of the neuron is behind that spot</t>
+  </si>
+  <si>
+    <t>How then can you calculate the probability that the neuron is behind the ___ square given it is not behind the ___ square?</t>
+  </si>
+  <si>
+    <t>This is a question of Conditional probability</t>
+  </si>
+  <si>
+    <t>We will begin by using the first method: P(A|B) = P(AnB)/P(B)</t>
+  </si>
+  <si>
+    <t>First lets calculate P(B) or the probability that the neuron is not behind this square</t>
+  </si>
+  <si>
+    <t>Using what we learned about set theory we can say that P(B) = 1 - P(B')</t>
+  </si>
+  <si>
+    <t>What is the probability that the neuron IS behind the ___ square?</t>
+  </si>
+  <si>
+    <t>What are the locations where the axon hillock can exist?</t>
+  </si>
+  <si>
+    <t>How many of these locations incorporate the ___ square into the neuron?</t>
+  </si>
+  <si>
+    <t>Well Done on the last Level!</t>
+  </si>
+  <si>
+    <t>This level will introduce Conditional Probability. But first some spatial reasoning questions!</t>
+  </si>
+  <si>
+    <t>Given the the neuron at the top right is fully hidden in this board and oriented as shown, behind which of the electrodes can the axon hillock exist? Click the squares, correct guesses will change color.</t>
+  </si>
+  <si>
+    <t>Now onto Conditional Probability</t>
   </si>
 </sst>
 </file>
@@ -811,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -856,10 +910,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -872,10 +926,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -910,10 +964,10 @@
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -926,10 +980,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -942,10 +996,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -958,10 +1012,10 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -992,90 +1046,90 @@
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>95</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -1084,10 +1138,10 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1104,10 +1158,10 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
@@ -1116,13 +1170,13 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="1"/>
@@ -1138,10 +1192,10 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -1150,13 +1204,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1164,13 +1218,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1178,13 +1232,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1192,10 +1246,10 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
@@ -1204,10 +1258,10 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
@@ -1216,30 +1270,30 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -1254,36 +1308,38 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -1292,32 +1348,32 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E36" s="3"/>
       <c r="F36" s="1"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="1"/>
@@ -1332,7 +1388,7 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1342,86 +1398,86 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="D40" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="1"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="1"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="7" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -1430,10 +1486,10 @@
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -1475,10 +1531,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1489,115 +1545,281 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>54</v>
+      <c r="A4" s="9" t="s">
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>56</v>
+      <c r="A5" s="9" t="s">
+        <v>124</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>57</v>
+        <v>93</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A9" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-    </row>
-    <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-    </row>
-    <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-    </row>
-    <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-    </row>
-    <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
     </row>
-    <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1608,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1622,16 +1844,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
@@ -1654,10 +1876,10 @@
     </row>
     <row r="4" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -1666,10 +1888,10 @@
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -1678,10 +1900,10 @@
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -1689,7 +1911,9 @@
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -1698,7 +1922,7 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -1707,7 +1931,9 @@
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -1716,9 +1942,11 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="11"/>
+        <v>61</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -1726,90 +1954,307 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B11" s="11"/>
+        <v>62</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B12" s="11"/>
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="A13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
+      <c r="A14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
+      <c r="A15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
+      <c r="A16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="A17" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="A18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>105</v>
+      </c>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
       <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
     </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="11"/>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11"/>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11"/>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="11"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
excel: typo & "enter key" to continue button"
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Documents\MATLAB\NDA_final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Becca\Documents\GitHub\NDA_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
@@ -49,18 +49,12 @@
     <t>You have been assigned to take on the mission of location where our battleship is.</t>
   </si>
   <si>
-    <t>Here you will see how to play and interact with the game. Go ahead, press the enter key.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
     <t>Press the enter key on your keyboard.</t>
   </si>
   <si>
-    <t>Good job! If you need any help, just press the hint button on the righ in the Notebook. Try it now.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>I am the 1st hint, press the hint key again</t>
   </si>
   <si>
-    <t>I am the 2nd hint. Now press the enter key.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @probArry</t>
   </si>
   <si>
@@ -479,6 +470,15 @@
   </si>
   <si>
     <t>Given the neuron is fully hidden in this board and oriented as shown, behind which of the electrodes can the axon hillock exist? Click the squares, correct guesses will change color.</t>
+  </si>
+  <si>
+    <t>Here you will see how to play and interact with the game. Go ahead, press the continue button.</t>
+  </si>
+  <si>
+    <t>Good job! If you need any help, just press the hint button on the right in the Notebook. Try it now.</t>
+  </si>
+  <si>
+    <t>I am the 2nd hint. Now press the continue button.</t>
   </si>
 </sst>
 </file>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1003,10 +1003,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -1019,10 +1019,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
@@ -1037,13 +1037,13 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1051,64 +1051,64 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>10</v>
+        <v>149</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>75</v>
+        <v>150</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1123,106 +1123,106 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1251,10 +1251,10 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
@@ -1263,13 +1263,13 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="9"/>
@@ -1285,10 +1285,10 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1297,13 +1297,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1311,13 +1311,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1325,13 +1325,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1339,10 +1339,10 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1351,10 +1351,10 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1363,30 +1363,30 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
@@ -1401,37 +1401,37 @@
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1441,39 +1441,39 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1493,86 +1493,86 @@
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="D40" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
@@ -1581,10 +1581,10 @@
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
@@ -1628,7 +1628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1642,376 +1642,376 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="C20" s="7" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>143</v>
-      </c>
       <c r="C27" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2041,16 +2041,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -2073,10 +2073,10 @@
     </row>
     <row r="4" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -2085,10 +2085,10 @@
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2097,10 +2097,10 @@
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2119,7 +2119,7 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2129,7 +2129,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2139,10 +2139,10 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2151,10 +2151,10 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2163,10 +2163,10 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2175,10 +2175,10 @@
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2187,10 +2187,10 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2199,10 +2199,10 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2211,10 +2211,10 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2223,10 +2223,10 @@
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2235,10 +2235,10 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2247,10 +2247,10 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2259,10 +2259,10 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2271,170 +2271,170 @@
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
first few medium questions running
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="153">
   <si>
     <t>question</t>
   </si>
@@ -367,9 +367,6 @@
     <t>We will practice calculating the conditional probabilty using both methods to show their equivalence</t>
   </si>
   <si>
-    <t>Do you see the ___ square on the board? This color denotes that no part of the neuron is behind that spot</t>
-  </si>
-  <si>
     <t>This is a question of Conditional probability</t>
   </si>
   <si>
@@ -400,12 +397,6 @@
     <t>Now onto Conditional Probability!</t>
   </si>
   <si>
-    <t>How can you calculate the probability that part of neuron is behind the ___ square given that no part is behind the ___ square?</t>
-  </si>
-  <si>
-    <t>What is the probability that the neuron IS behind the ___ square and not behind the ___ square?</t>
-  </si>
-  <si>
     <t xml:space="preserve">How many locations is the include the ___ square and not the ___ square? </t>
   </si>
   <si>
@@ -421,9 +412,6 @@
     <t>As a reminder Bayes Rule states that: P(A|B) = P(B/A)*P(A)/P(B)</t>
   </si>
   <si>
-    <t>First lets calculate P(A) or the probability that the neuron IS behind the ____ square</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @probBehind1</t>
   </si>
   <si>
@@ -433,15 +421,9 @@
     <t>Do you remember what P(B) was?</t>
   </si>
   <si>
-    <t>What is the probability that the neuron is NOT behind the ___ square?</t>
-  </si>
-  <si>
     <t>1 - P(B)</t>
   </si>
   <si>
-    <t>What is the probability that the neuron IS behind the ___ square? (write this number down)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @probNotBehind1</t>
   </si>
   <si>
@@ -481,7 +463,28 @@
     <t>Given the neuron is fully hidden in this board and oriented as shown…</t>
   </si>
   <si>
-    <t>Behind which of the electrodes can the axon hillock exist? Double click the electrode squares. Correct guesses will change color. Answer 'Go' to begin.</t>
+    <t>Behind which of the electrodes can the axon hillock exist? Quadruple click the electrode squares (Builds character!) Correct guesses will change color. Answer 'Go' to begin.</t>
+  </si>
+  <si>
+    <t>Do you see the jade square on the board? This color denotes that no part of the neuron is behind that spot</t>
+  </si>
+  <si>
+    <t>How can you calculate the probability that part of neuron is behind the lilac square given that no part is behind the jade square?</t>
+  </si>
+  <si>
+    <t>What is the probability that the neuron IS behind the jade square? (write this number down)</t>
+  </si>
+  <si>
+    <t>What is the probability that the neuron is NOT behind the jade square?</t>
+  </si>
+  <si>
+    <t>What is the probability that the neuron IS behind the lilac square and not behind the jade square?</t>
+  </si>
+  <si>
+    <t>What is the probability that the neuron is behind the lilac square given it is not behind the jade square?</t>
+  </si>
+  <si>
+    <t>First lets calculate P(A) or the probability that the neuron IS behind the lilac square</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1479,7 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1631,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1671,7 +1674,7 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>63</v>
@@ -1685,7 +1688,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>63</v>
@@ -1699,7 +1702,7 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>63</v>
@@ -1713,7 +1716,7 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>93</v>
@@ -1730,7 +1733,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>53</v>
@@ -1741,13 +1744,21 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>113</v>
+        <v>146</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>63</v>
@@ -1761,7 +1772,7 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>63</v>
@@ -1775,7 +1786,7 @@
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>63</v>
@@ -1859,7 +1870,7 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>63</v>
@@ -1873,7 +1884,7 @@
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>63</v>
@@ -1887,7 +1898,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>63</v>
@@ -1901,16 +1912,16 @@
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>63</v>
@@ -1918,62 +1929,62 @@
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>63</v>
@@ -1981,7 +1992,7 @@
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>63</v>
@@ -1995,40 +2006,40 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the language in questions excel file
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Documents\MATLAB\NDA_final_project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
     <sheet name="medium" sheetId="2" r:id="rId2"/>
     <sheet name="hard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -49,18 +44,12 @@
     <t>You have been assigned to take on the mission of location where our battleship is.</t>
   </si>
   <si>
-    <t>Here you will see how to play and interact with the game. Go ahead, press the enter key.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
     <t>Press the enter key on your keyboard.</t>
   </si>
   <si>
-    <t>Good job! If you need any help, just press the hint button on the righ in the Notebook. Try it now.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
@@ -253,9 +242,6 @@
     <t>I am the 1st hint, press the hint key again</t>
   </si>
   <si>
-    <t>I am the 2nd hint. Now press the enter key.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @probArry</t>
   </si>
   <si>
@@ -485,6 +471,15 @@
   </si>
   <si>
     <t>First lets calculate P(A) or the probability that the neuron IS behind the lilac square</t>
+  </si>
+  <si>
+    <t>Here you will see how to play and interact with the game. Go ahead, press the continue key.</t>
+  </si>
+  <si>
+    <t>Good job! If you need any help, just press the hint button on the right. Try it now.</t>
+  </si>
+  <si>
+    <t>I am the 2nd hint. Now press the continue key.</t>
   </si>
 </sst>
 </file>
@@ -963,21 +958,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="151.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" style="7" customWidth="1"/>
-    <col min="5" max="6" width="13.85546875" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="17.28515625" style="7"/>
+    <col min="1" max="1" width="151.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="7" customWidth="1"/>
+    <col min="5" max="6" width="13.83203125" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="17.33203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -993,7 +988,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1001,7 +996,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -1009,15 +1004,15 @@
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
@@ -1025,15 +1020,15 @@
         <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1041,85 +1036,85 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>75</v>
+        <v>152</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
@@ -1127,127 +1122,127 @@
       <c r="E11" s="10"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>19</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
@@ -1255,33 +1250,33 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1289,115 +1284,115 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>31</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>33</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1405,39 +1400,39 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1445,41 +1440,41 @@
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1487,9 +1482,9 @@
       <c r="E38" s="11"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1497,105 +1492,105 @@
       <c r="E39" s="11"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="D40" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="14" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -1603,7 +1598,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="10"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -1611,7 +1606,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -1621,7 +1616,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1634,417 +1629,417 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="118.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="7" customWidth="1"/>
-    <col min="3" max="6" width="13.42578125" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="17.28515625" style="7"/>
+    <col min="1" max="1" width="118.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="7" customWidth="1"/>
+    <col min="3" max="6" width="13.5" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="17.33203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1">
+      <c r="A8" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="B8" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1">
+      <c r="A9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1">
+      <c r="A10" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1">
+      <c r="A11" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1">
+      <c r="A12" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1">
+      <c r="A13" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1">
+      <c r="A14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1">
+      <c r="A15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1">
+      <c r="A16" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1">
+      <c r="A17" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1">
+      <c r="A18" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="A19" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1">
+      <c r="A20" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="A22" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1">
+      <c r="A23" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1">
+      <c r="A24" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1">
+      <c r="A25" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1">
+      <c r="A26" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1">
+      <c r="A27" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B23" s="7" t="s">
+      <c r="B29" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A31" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2061,29 +2056,29 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="143.140625" customWidth="1"/>
-    <col min="2" max="6" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="143.1640625" customWidth="1"/>
+    <col min="2" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2091,7 +2086,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2099,45 +2094,45 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2145,9 +2140,9 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2155,9 +2150,9 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2165,321 +2160,321 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1">
       <c r="B45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
almost finished med question
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="152">
   <si>
     <t>question</t>
   </si>
@@ -403,51 +403,27 @@
     <t>P(A|B) = P(AnB)/P(B)</t>
   </si>
   <si>
-    <t>What is the probability that the neuron is behind the ___ square given it is not behind the ____ square?</t>
-  </si>
-  <si>
     <t>Now we will calculate the same value using Bayes Rule</t>
   </si>
   <si>
     <t>As a reminder Bayes Rule states that: P(A|B) = P(B/A)*P(A)/P(B)</t>
   </si>
   <si>
-    <t xml:space="preserve"> @probBehind1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> @probBehind2</t>
-  </si>
-  <si>
     <t>Do you remember what P(B) was?</t>
   </si>
   <si>
     <t>1 - P(B)</t>
   </si>
   <si>
-    <t xml:space="preserve"> @probNotBehind1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> @probNotBehind2</t>
-  </si>
-  <si>
-    <t>What is the probability that the neuron is not behind the ___ square given it is behind the ___ square?</t>
-  </si>
-  <si>
     <t>How many ways can part of the neuron be behind the ____ square?</t>
   </si>
   <si>
     <t>Of these what percentage do not include part of the nueron behind the ____ square?</t>
   </si>
   <si>
-    <t xml:space="preserve"> @probNotBehind3</t>
-  </si>
-  <si>
     <t>P(A|B) = P(B/A)*P(A)/P(B)</t>
   </si>
   <si>
-    <t xml:space="preserve"> @conditional</t>
-  </si>
-  <si>
     <t>Were the values found using the definition and by using Bayes Rule the same?</t>
   </si>
   <si>
@@ -472,9 +448,6 @@
     <t>How can you calculate the probability that part of neuron is behind the lilac square given that no part is behind the jade square?</t>
   </si>
   <si>
-    <t>What is the probability that the neuron IS behind the jade square? (write this number down)</t>
-  </si>
-  <si>
     <t>What is the probability that the neuron is NOT behind the jade square?</t>
   </si>
   <si>
@@ -485,6 +458,30 @@
   </si>
   <si>
     <t>First lets calculate P(A) or the probability that the neuron IS behind the lilac square</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the probability that the neuron IS behind the jade square? </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @seven25ths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @eighteen25ths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @four25ths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @two9ths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @six25ths</t>
+  </si>
+  <si>
+    <t>What is the probability that the neuron is not behind the jade square given it is behind the lilac square?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @four6ths</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1476,7 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1634,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1702,7 +1699,7 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>63</v>
@@ -1716,7 +1713,7 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>93</v>
@@ -1747,7 +1744,7 @@
         <v>122</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>63</v>
@@ -1758,10 +1755,10 @@
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>63</v>
@@ -1772,10 +1769,10 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>63</v>
@@ -1789,7 +1786,7 @@
         <v>113</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>63</v>
@@ -1803,7 +1800,7 @@
         <v>108</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>63</v>
@@ -1817,7 +1814,7 @@
         <v>109</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>63</v>
@@ -1831,7 +1828,7 @@
         <v>110</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>63</v>
@@ -1845,7 +1842,7 @@
         <v>111</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>63</v>
@@ -1859,7 +1856,7 @@
         <v>112</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>63</v>
@@ -1873,7 +1870,7 @@
         <v>114</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>63</v>
@@ -1887,7 +1884,7 @@
         <v>115</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>63</v>
@@ -1901,7 +1898,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>63</v>
@@ -1912,10 +1909,10 @@
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>117</v>
@@ -1929,21 +1926,24 @@
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>117</v>
@@ -1954,31 +1954,52 @@
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>124</v>
       </c>
+      <c r="D23" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>117</v>
@@ -1992,10 +2013,10 @@
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>63</v>
@@ -2006,40 +2027,46 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>141</v>
+        <v>133</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Typos in excel easy sheet
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Documents\MATLAB\NDA_final_project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
     <sheet name="medium" sheetId="2" r:id="rId2"/>
     <sheet name="hard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -961,7 +956,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
edited the easy level funcs
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -260,9 +260,6 @@
     <t>If you have a set S containing an event w, we would say w is an element of S</t>
   </si>
   <si>
-    <t>Here we have an electrode array or a set E. It is composed of 64 electrodes or objects e. So e is an element E.</t>
-  </si>
-  <si>
     <t>The neuron is modelled in color at the top right corner of this figure.</t>
   </si>
   <si>
@@ -480,6 +477,9 @@
   </si>
   <si>
     <t>I am the 2nd hint. Now press the continue key.</t>
+  </si>
+  <si>
+    <t>Here we have an electrode array or a set E. It is composed of 49 electrodes or objects e. So e is an element E.</t>
   </si>
 </sst>
 </file>
@@ -959,7 +959,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1038,7 +1038,7 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>7</v>
@@ -1052,7 +1052,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>9</v>
@@ -1061,7 +1061,7 @@
         <v>72</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>79</v>
+        <v>152</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>21</v>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>73</v>
@@ -1188,7 +1188,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>24</v>
@@ -1220,7 +1220,7 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>64</v>
@@ -1232,7 +1232,7 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>74</v>
@@ -1252,7 +1252,7 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>64</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>62</v>
@@ -1298,13 +1298,13 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
@@ -1312,13 +1312,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>67</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1442,7 +1442,7 @@
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="10" t="s">
         <v>36</v>
@@ -1474,7 +1474,7 @@
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9" t="s">
@@ -1552,7 +1552,7 @@
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
@@ -1570,7 +1570,7 @@
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>61</v>
@@ -1669,7 +1669,7 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>61</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>61</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>61</v>
@@ -1711,10 +1711,10 @@
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>61</v>
@@ -1728,7 +1728,7 @@
         <v>50</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>51</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>61</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>61</v>
@@ -1767,7 +1767,7 @@
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>61</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>61</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>61</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>61</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>61</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>61</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>61</v>
@@ -1865,7 +1865,7 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>61</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>61</v>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>61</v>
@@ -1907,16 +1907,16 @@
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>61</v>
@@ -1924,62 +1924,62 @@
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C26" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>61</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>61</v>
@@ -2001,40 +2001,40 @@
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="D28" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2096,7 @@
     </row>
     <row r="4" spans="1:6" ht="30.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>56</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>57</v>
@@ -2120,7 +2120,7 @@
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>58</v>
@@ -2132,7 +2132,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2152,7 +2152,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2165,7 +2165,7 @@
         <v>59</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2177,7 +2177,7 @@
         <v>60</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2189,7 +2189,7 @@
         <v>59</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2201,7 +2201,7 @@
         <v>60</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2213,7 +2213,7 @@
         <v>59</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2225,7 +2225,7 @@
         <v>60</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2237,7 +2237,7 @@
         <v>59</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2249,7 +2249,7 @@
         <v>60</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2261,7 +2261,7 @@
         <v>59</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2273,7 +2273,7 @@
         <v>60</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -2285,7 +2285,7 @@
         <v>59</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2297,7 +2297,7 @@
         <v>60</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
@@ -2305,7 +2305,7 @@
         <v>59</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
@@ -2313,7 +2313,7 @@
         <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
@@ -2321,7 +2321,7 @@
         <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
@@ -2329,7 +2329,7 @@
         <v>60</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
@@ -2337,7 +2337,7 @@
         <v>59</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
@@ -2345,7 +2345,7 @@
         <v>60</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
@@ -2353,7 +2353,7 @@
         <v>59</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
@@ -2361,7 +2361,7 @@
         <v>60</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
@@ -2369,7 +2369,7 @@
         <v>59</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
@@ -2377,7 +2377,7 @@
         <v>60</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
@@ -2385,7 +2385,7 @@
         <v>59</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" customHeight="1">
@@ -2393,7 +2393,7 @@
         <v>60</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" customHeight="1">
@@ -2401,7 +2401,7 @@
         <v>59</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" customHeight="1">
@@ -2409,7 +2409,7 @@
         <v>60</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" customHeight="1">
@@ -2417,7 +2417,7 @@
         <v>59</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" customHeight="1">
@@ -2425,7 +2425,7 @@
         <v>60</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" customHeight="1">
@@ -2433,7 +2433,7 @@
         <v>59</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" customHeight="1">
@@ -2441,7 +2441,7 @@
         <v>60</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" customHeight="1">
@@ -2449,7 +2449,7 @@
         <v>59</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" customHeight="1">
@@ -2457,7 +2457,7 @@
         <v>60</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
let's try this again
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21900" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
@@ -41,21 +41,12 @@
     <t>@KeyPressed</t>
   </si>
   <si>
-    <t>You have been assigned to take on the mission of location where our battleship is.</t>
-  </si>
-  <si>
-    <t>Here you will see how to play and interact with the game. Go ahead, press the enter key.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
     <t>Press the enter key on your keyboard.</t>
   </si>
   <si>
-    <t>Good job! If you need any help, just press the hint button on the righ in the Notebook. Try it now.</t>
-  </si>
-  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
@@ -245,12 +236,6 @@
     <t>Our neuron is composed of dendrites (D), axons (A), and a axon hillock (AH).</t>
   </si>
   <si>
-    <t>I am the 1st hint, press the hint key again</t>
-  </si>
-  <si>
-    <t>I am the 2nd hint. Now press the enter key.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> @probArry</t>
   </si>
   <si>
@@ -477,6 +462,21 @@
   </si>
   <si>
     <t>Here we have an electrode array or a set E. It is composed of 49 electrodes or objects e. So e is an element E.</t>
+  </si>
+  <si>
+    <t>Here you will see how to play and interact with the game. Go ahead, press the continue button.</t>
+  </si>
+  <si>
+    <t>You have been assigned  the mission of locating where our battleship is.</t>
+  </si>
+  <si>
+    <t>Good job! If you need any help, just press the hint button on the right in the Notebook. Try it now.</t>
+  </si>
+  <si>
+    <t>I am the 1st hint, press the hint button again</t>
+  </si>
+  <si>
+    <t>I am the 2nd hint. Now press the continue button.</t>
   </si>
 </sst>
 </file>
@@ -956,20 +956,20 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="151.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="7" customWidth="1"/>
-    <col min="5" max="6" width="13.83203125" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="7"/>
+    <col min="1" max="1" width="151.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" style="7" customWidth="1"/>
+    <col min="5" max="6" width="13.85546875" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -985,7 +985,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -993,7 +993,7 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1">
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -1001,31 +1001,31 @@
         <v>5</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1">
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1033,85 +1033,85 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>10</v>
+        <v>149</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>74</v>
+        <v>150</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
@@ -1119,127 +1119,127 @@
       <c r="E11" s="10"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>21</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="9"/>
@@ -1247,33 +1247,33 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="19.5" customHeight="1">
+    <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D22" s="11"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -1281,115 +1281,115 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1">
+    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1">
+    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1">
+    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1">
+    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1">
+    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1">
+    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1397,39 +1397,39 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1">
+    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B33" s="11"/>
       <c r="C33" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1">
+    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1">
+    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -1437,41 +1437,41 @@
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1">
+    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1">
+    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1">
+    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1479,9 +1479,9 @@
       <c r="E38" s="11"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1">
+    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1489,105 +1489,105 @@
       <c r="E39" s="11"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1">
+    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1">
+    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="14" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1">
+    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1">
+    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1">
+    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1">
+    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1">
+    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -1595,7 +1595,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1">
+    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10"/>
       <c r="B48" s="11"/>
       <c r="C48" s="11"/>
@@ -1603,7 +1603,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1">
+    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
@@ -1630,438 +1630,438 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="118.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="7" customWidth="1"/>
-    <col min="3" max="6" width="13.5" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="17.33203125" style="7"/>
+    <col min="1" max="1" width="118.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="7" customWidth="1"/>
+    <col min="3" max="6" width="13.42578125" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="17.28515625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="C9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1">
-      <c r="A3" s="6" t="s">
+      <c r="C10" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="D23" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C24" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1">
-      <c r="A4" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
-      <c r="A6" s="6" t="s">
+      <c r="C25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1">
-      <c r="A7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
-      <c r="A9" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1">
-      <c r="A10" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1">
-      <c r="A11" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1">
-      <c r="A12" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1">
-      <c r="A14" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1">
-      <c r="A15" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1">
-      <c r="A16" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
-      <c r="A17" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
-      <c r="A18" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
-      <c r="A19" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
-      <c r="A20" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1">
-      <c r="A21" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B29" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1">
-      <c r="A23" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1">
-      <c r="A24" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1">
-      <c r="A25" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1">
-      <c r="A26" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1">
-      <c r="A27" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A28" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C28" s="7" t="s">
+      <c r="C30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
         <v>128</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A29" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A30" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A31" s="8" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2083,29 +2083,29 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="143.1640625" customWidth="1"/>
-    <col min="2" max="6" width="13.83203125" customWidth="1"/>
+    <col min="1" max="1" width="143.140625" customWidth="1"/>
+    <col min="2" max="6" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1">
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2113,7 +2113,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2121,45 +2121,45 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="30.75" customHeight="1">
+    <row r="4" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1">
+    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="30.75" customHeight="1">
+    <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1">
+    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2167,9 +2167,9 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1">
+    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2177,9 +2177,9 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1">
+    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2187,316 +2187,316 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1">
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1">
+    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1">
+    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1">
+    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1">
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1">
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="15.75" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="15.75" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:2" ht="15.75" customHeight="1">
+    <row r="43" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="1:2" ht="15.75" customHeight="1">
+    <row r="44" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:2" ht="15.75" customHeight="1">
+    <row r="45" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed some excel typos that were reverted
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivana\Documents\MATLAB\NDA_final_project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
     <sheet name="medium" sheetId="2" r:id="rId2"/>
     <sheet name="hard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -451,15 +446,9 @@
     <t>Welcome to USS Sampson's Neuron Battleship!  {Press Continue}</t>
   </si>
   <si>
-    <t>You have been assigned to take on the mission of location where our battleship is.  {Press Continue}</t>
-  </si>
-  <si>
     <t>Here you will see how to play and interact with the game.  {Press Continue}</t>
   </si>
   <si>
-    <t>Good job! If you need any help, just press the hint button on the righ in the Notebook. Try it now.  {Press Hint}</t>
-  </si>
-  <si>
     <t>I am the 2nd hint. Now press continue.</t>
   </si>
   <si>
@@ -481,9 +470,6 @@
     <t>The law of total probability states that the total probability of all events in a set is 1.  {Press Continue}</t>
   </si>
   <si>
-    <t>Here we have an electrode array or a set E. It is composed of 64 electrodes or objects e. So e is an element E.  {Press Continue}</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Now lets learn about our neuron.  {Press Continue}</t>
   </si>
   <si>
@@ -515,6 +501,15 @@
   </si>
   <si>
     <t>Independence means there is thte occurance of one event has no bearing on the possibility of occurance for the other. Numerically, two events are independent if and only if P(AnB) = P(A) P(B).  {Press Continue}</t>
+  </si>
+  <si>
+    <t>You have been assigned the mission of locating where our battleship is.  {Press Continue}</t>
+  </si>
+  <si>
+    <t>Good job! If you need any help, just press the hint button on the right in the Notebook. Try it now.  {Press Hint}</t>
+  </si>
+  <si>
+    <t>Here we have an electrode array or a set E. It is composed of 49 electrodes or objects e. So e is an element E.  {Press Continue}</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1069,7 +1064,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>133</v>
@@ -1085,7 +1080,7 @@
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>134</v>
@@ -1115,7 +1110,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>7</v>
@@ -1124,14 +1119,14 @@
         <v>60</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>8</v>
@@ -1147,7 +1142,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
@@ -1163,7 +1158,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>10</v>
@@ -1187,7 +1182,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
@@ -1203,7 +1198,7 @@
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>14</v>
@@ -1219,7 +1214,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>55</v>
@@ -1235,7 +1230,7 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>15</v>
@@ -1267,7 +1262,7 @@
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>18</v>
@@ -1283,7 +1278,7 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>4</v>
@@ -1299,7 +1294,7 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>55</v>
@@ -1331,7 +1326,7 @@
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>55</v>
@@ -1365,7 +1360,7 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>19</v>
@@ -1377,7 +1372,7 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>20</v>
@@ -1391,7 +1386,7 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>21</v>
@@ -1405,7 +1400,7 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>22</v>
@@ -1419,7 +1414,7 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>55</v>
@@ -1431,7 +1426,7 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>55</v>
@@ -1521,7 +1516,7 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>28</v>
@@ -2184,7 +2179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" workbookViewId="0">
+    <sheetView topLeftCell="B30" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
modified fun tion types for easy level
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23620" windowHeight="14240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
     <sheet name="medium" sheetId="2" r:id="rId2"/>
     <sheet name="hard" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="160">
   <si>
     <t>question</t>
   </si>
@@ -192,9 +192,6 @@
   </si>
   <si>
     <t xml:space="preserve"> @anrYes</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> @prob</t>
   </si>
   <si>
     <t>If you choose a square at random from the neuron, what is the probability of choosing the axon hillock or axon?</t>
@@ -511,12 +508,18 @@
   <si>
     <t>Here we have an electrode array or a set E. It is composed of 49 electrodes or objects e. So e is an element E.  {Press Continue}</t>
   </si>
+  <si>
+    <t xml:space="preserve"> @probAxonAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @probDendriteAH</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -574,6 +577,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -620,8 +635,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -668,7 +685,9 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1009,20 +1028,20 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="151.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" style="7" customWidth="1"/>
-    <col min="5" max="6" width="13.85546875" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="17.28515625" style="7"/>
+    <col min="1" max="1" width="151.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="50.5" style="7" customWidth="1"/>
+    <col min="5" max="6" width="13.83203125" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="17.33203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1057,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1046,9 +1065,9 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>4</v>
@@ -1062,12 +1081,12 @@
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>52</v>
@@ -1078,12 +1097,12 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>52</v>
@@ -1094,9 +1113,9 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>5</v>
@@ -1108,25 +1127,25 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>8</v>
@@ -1140,9 +1159,9 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>9</v>
@@ -1156,9 +1175,9 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>10</v>
@@ -1172,7 +1191,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
@@ -1180,9 +1199,9 @@
       <c r="E11" s="10"/>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
@@ -1196,9 +1215,9 @@
       <c r="E12" s="11"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>14</v>
@@ -1212,9 +1231,9 @@
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>55</v>
@@ -1228,9 +1247,9 @@
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>15</v>
@@ -1244,12 +1263,12 @@
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>16</v>
@@ -1260,9 +1279,9 @@
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>18</v>
@@ -1276,9 +1295,9 @@
       <c r="E17" s="11"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>4</v>
@@ -1292,9 +1311,9 @@
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>55</v>
@@ -1304,19 +1323,19 @@
       <c r="E19" s="11"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="11"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="15" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="9"/>
@@ -1324,9 +1343,9 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
     </row>
-    <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="19.5" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>55</v>
@@ -1336,9 +1355,9 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>53</v>
@@ -1350,7 +1369,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="15" customHeight="1">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -1358,9 +1377,9 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>19</v>
@@ -1370,37 +1389,37 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
     </row>
-    <row r="28" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>22</v>
@@ -1412,9 +1431,9 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
     </row>
-    <row r="29" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>55</v>
@@ -1424,9 +1443,9 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
     </row>
-    <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>55</v>
@@ -1436,12 +1455,12 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
     </row>
-    <row r="31" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>57</v>
+        <v>158</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>24</v>
@@ -1452,11 +1471,13 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
-    <row r="32" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="9"/>
+        <v>58</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>159</v>
+      </c>
       <c r="C32" s="9" t="s">
         <v>25</v>
       </c>
@@ -1466,7 +1487,7 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="15" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -1474,7 +1495,7 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
     </row>
-    <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="9" t="s">
         <v>26</v>
       </c>
@@ -1488,9 +1509,9 @@
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
     </row>
-    <row r="35" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>56</v>
@@ -1504,9 +1525,9 @@
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
     </row>
-    <row r="36" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -1514,9 +1535,9 @@
       <c r="E36" s="11"/>
       <c r="F36" s="9"/>
     </row>
-    <row r="37" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>28</v>
@@ -1530,25 +1551,25 @@
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
     </row>
-    <row r="38" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="9"/>
     </row>
-    <row r="39" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -1556,7 +1577,7 @@
       <c r="E39" s="11"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15" customHeight="1">
       <c r="A40" s="9" t="s">
         <v>30</v>
       </c>
@@ -1566,7 +1587,7 @@
       <c r="E40" s="11"/>
       <c r="F40" s="9"/>
     </row>
-    <row r="41" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15" customHeight="1">
       <c r="A41" s="10" t="s">
         <v>31</v>
       </c>
@@ -1582,7 +1603,7 @@
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
     </row>
-    <row r="42" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15" customHeight="1">
       <c r="A42" s="14" t="s">
         <v>34</v>
       </c>
@@ -1596,7 +1617,7 @@
       <c r="E42" s="11"/>
       <c r="F42" s="9"/>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15" customHeight="1">
       <c r="A43" s="14" t="s">
         <v>36</v>
       </c>
@@ -1610,9 +1631,9 @@
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
-    <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15" customHeight="1">
       <c r="A44" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9" t="s">
@@ -1624,9 +1645,9 @@
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
-    <row r="45" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15" customHeight="1">
       <c r="A45" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="9" t="s">
@@ -1638,13 +1659,13 @@
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
     </row>
-    <row r="46" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15" customHeight="1">
       <c r="A46" s="14" t="s">
         <v>37</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>52</v>
@@ -1652,7 +1673,7 @@
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
     </row>
-    <row r="47" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15" customHeight="1">
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9" t="s">
@@ -1664,7 +1685,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
     </row>
-    <row r="48" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15" customHeight="1">
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
@@ -1672,7 +1693,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="9"/>
     </row>
-    <row r="49" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15" customHeight="1">
       <c r="A49" s="10"/>
       <c r="B49" s="11"/>
       <c r="C49" s="11"/>
@@ -1680,7 +1701,7 @@
       <c r="E49" s="9"/>
       <c r="F49" s="9"/>
     </row>
-    <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15" customHeight="1">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -1690,7 +1711,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1707,15 +1728,15 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="118.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" style="7" customWidth="1"/>
-    <col min="3" max="6" width="13.42578125" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="17.28515625" style="7"/>
+    <col min="1" max="1" width="118.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" style="7" customWidth="1"/>
+    <col min="3" max="6" width="13.5" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="17.33203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>38</v>
       </c>
@@ -1729,7 +1750,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>52</v>
@@ -1741,68 +1762,68 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
+      <c r="A6" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1">
+      <c r="A7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>42</v>
@@ -1811,9 +1832,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>55</v>
@@ -1825,9 +1846,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>55</v>
@@ -1839,9 +1860,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>55</v>
@@ -1853,9 +1874,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>55</v>
@@ -1867,9 +1888,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>55</v>
@@ -1881,9 +1902,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>55</v>
@@ -1895,9 +1916,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>55</v>
@@ -1909,9 +1930,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>55</v>
@@ -1923,9 +1944,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>55</v>
@@ -1937,9 +1958,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>55</v>
@@ -1951,9 +1972,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>55</v>
@@ -1965,9 +1986,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>55</v>
@@ -1979,68 +2000,68 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" customHeight="1">
+      <c r="A21" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="C21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="A22" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="C22" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1">
+      <c r="A23" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>90</v>
-      </c>
       <c r="D23" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>55</v>
@@ -2052,9 +2073,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>55</v>
@@ -2066,69 +2087,69 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1">
+      <c r="A27" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="7" t="s">
-        <v>111</v>
-      </c>
       <c r="C28" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="7" t="s">
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C29" s="7" t="s">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>97</v>
-      </c>
       <c r="C30" s="7" t="s">
         <v>52</v>
       </c>
@@ -2136,9 +2157,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>55</v>
@@ -2150,9 +2171,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>4</v>
@@ -2166,7 +2187,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2183,13 +2204,13 @@
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="143.140625" customWidth="1"/>
-    <col min="2" max="6" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="143.1640625" customWidth="1"/>
+    <col min="2" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
@@ -2205,7 +2226,7 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -2213,7 +2234,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -2221,9 +2242,9 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>47</v>
@@ -2237,9 +2258,9 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>48</v>
@@ -2253,9 +2274,9 @@
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>49</v>
@@ -2269,9 +2290,9 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="17" t="s">
@@ -2283,9 +2304,9 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="17" t="s">
@@ -2297,9 +2318,9 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="17" t="s">
@@ -2311,12 +2332,12 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>52</v>
@@ -2327,12 +2348,12 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>52</v>
@@ -2343,12 +2364,12 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>52</v>
@@ -2359,12 +2380,12 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>52</v>
@@ -2375,12 +2396,12 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>52</v>
@@ -2391,12 +2412,12 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>52</v>
@@ -2407,12 +2428,12 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>52</v>
@@ -2423,12 +2444,12 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>52</v>
@@ -2439,12 +2460,12 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>52</v>
@@ -2455,12 +2476,12 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>52</v>
@@ -2471,12 +2492,12 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>52</v>
@@ -2487,12 +2508,12 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>52</v>
@@ -2501,12 +2522,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>52</v>
@@ -2515,12 +2536,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>52</v>
@@ -2529,12 +2550,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="17" t="s">
         <v>52</v>
@@ -2543,12 +2564,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>52</v>
@@ -2557,12 +2578,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>52</v>
@@ -2571,12 +2592,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>52</v>
@@ -2585,12 +2606,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>52</v>
@@ -2599,12 +2620,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>52</v>
@@ -2613,12 +2634,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>52</v>
@@ -2627,12 +2648,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>52</v>
@@ -2641,12 +2662,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>52</v>
@@ -2655,12 +2676,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="17" t="s">
         <v>52</v>
@@ -2669,12 +2690,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>52</v>
@@ -2683,12 +2704,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>52</v>
@@ -2697,12 +2718,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>52</v>
@@ -2711,12 +2732,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>52</v>
@@ -2725,12 +2746,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>52</v>
@@ -2739,12 +2760,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>52</v>
@@ -2753,12 +2774,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>52</v>
@@ -2767,12 +2788,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>52</v>
@@ -2781,21 +2802,21 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1">
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1">
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.75" customHeight="1">
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1">
       <c r="B45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
edited easy level questions
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23620" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26360" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="easy" sheetId="1" r:id="rId1"/>
     <sheet name="medium" sheetId="2" r:id="rId2"/>
     <sheet name="hard" sheetId="3" r:id="rId3"/>
+    <sheet name="extra concepts" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="146">
   <si>
     <t>question</t>
   </si>
@@ -38,10 +39,88 @@
     <t>@KeyPressed</t>
   </si>
   <si>
+    <t>Press the enter key on your keyboard.</t>
+  </si>
+  <si>
+    <t>Example: coin flip. S={H,T}.</t>
+  </si>
+  <si>
+    <t>Example: dice roll. S={1,2,3,4,5,6}.</t>
+  </si>
+  <si>
+    <t>P(E)</t>
+  </si>
+  <si>
+    <t>How many electrodes are in the electrode array?</t>
+  </si>
+  <si>
+    <t>Example: A be the event that roll is odd and B be the event that the roll is even. Here A and B are disjoint.</t>
+  </si>
+  <si>
+    <t>P(AH) + P(A)</t>
+  </si>
+  <si>
+    <t>P(AH) + P(D)</t>
+  </si>
+  <si>
+    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon or dendrite?</t>
+  </si>
+  <si>
+    <t>P(A) + P(D)</t>
+  </si>
+  <si>
+    <t>P(A) ⊥ P(D)</t>
+  </si>
+  <si>
+    <t>Concepts to implement still:</t>
+  </si>
+  <si>
+    <t>If you have 2 sets, A and B, and set B fully encompasses set A, then set A is considered to be a subset of B.</t>
+  </si>
+  <si>
     <t>@KeyPressed</t>
   </si>
   <si>
-    <t>Press the enter key on your keyboard.</t>
+    <t>A ⊆ B</t>
+  </si>
+  <si>
+    <t>P(A)≤1</t>
+  </si>
+  <si>
+    <t>A ∪ B = B ∪ A.</t>
+  </si>
+  <si>
+    <t>P(Ac)=1-P(A), where Ac is the complement of A</t>
+  </si>
+  <si>
+    <t>Law of total probability</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>hint1</t>
+  </si>
+  <si>
+    <t>hint2</t>
+  </si>
+  <si>
+    <t>P(AH)</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>hint1</t>
+  </si>
+  <si>
+    <t>hint2</t>
   </si>
   <si>
     <t>@KeyPressed</t>
@@ -53,126 +132,6 @@
     <t>@KeyPressed</t>
   </si>
   <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>Example: coin flip. S={H,T}.</t>
-  </si>
-  <si>
-    <t>Example: dice roll. S={1,2,3,4,5,6}.</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>P(E)</t>
-  </si>
-  <si>
-    <t>How many electrodes are in the electrode array?</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>Example: A be the event that roll is odd and B be the event that the roll is even. Here A and B are disjoint.</t>
-  </si>
-  <si>
-    <t>P(AH) + P(A)</t>
-  </si>
-  <si>
-    <t>P(AH) + P(D)</t>
-  </si>
-  <si>
-    <t>If you choose a square at random from the electrode array, what is the probability of choosing the axon or dendrite?</t>
-  </si>
-  <si>
-    <t>P(A) + P(D)</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>P(A) ⊥ P(D)</t>
-  </si>
-  <si>
-    <t>Concepts to implement still:</t>
-  </si>
-  <si>
-    <t>If you have 2 sets, A and B, and set B fully encompasses set A, then set A is considered to be a subset of B.</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>A ⊆ B</t>
-  </si>
-  <si>
-    <t>P(A)≤1</t>
-  </si>
-  <si>
-    <t>A ∪ B = B ∪ A.</t>
-  </si>
-  <si>
-    <t>P(Ac)=1-P(A), where Ac is the complement of A</t>
-  </si>
-  <si>
-    <t>Law of total probability</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>answer</t>
-  </si>
-  <si>
-    <t>hint1</t>
-  </si>
-  <si>
-    <t>hint2</t>
-  </si>
-  <si>
-    <t>P(AH)</t>
-  </si>
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>answer</t>
-  </si>
-  <si>
-    <t>hint1</t>
-  </si>
-  <si>
-    <t>hint2</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
-    <t>@KeyPressed</t>
-  </si>
-  <si>
     <t>Where do you guess the neuron might be?</t>
   </si>
   <si>
@@ -419,24 +378,6 @@
     <t>Seriously?</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>@KeyPressed</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">  @KeyPressed</t>
-  </si>
-  <si>
     <t xml:space="preserve"> To submit an answer type it below and press Enter. Go ahead, type anything and press the enter key.</t>
   </si>
   <si>
@@ -513,13 +454,19 @@
   </si>
   <si>
     <t xml:space="preserve"> @probDendriteAH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @probAxonDendrite</t>
+  </si>
+  <si>
+    <t>Extra concepts:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -561,13 +508,6 @@
       <i/>
       <sz val="10"/>
       <color rgb="FF252525"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -635,10 +575,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -678,16 +626,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1027,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1067,61 +1023,61 @@
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>132</v>
+        <v>41</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>133</v>
+        <v>120</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B6" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>6</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1129,64 +1085,64 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="9" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
@@ -1201,122 +1157,122 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E12" s="11"/>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="9" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E18" s="11"/>
       <c r="F18" s="9"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>55</v>
+        <v>130</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1325,10 +1281,10 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1345,10 +1301,10 @@
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="10"/>
@@ -1357,13 +1313,13 @@
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1">
       <c r="A23" s="9" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="9"/>
@@ -1379,10 +1335,10 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -1391,13 +1347,13 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
@@ -1405,13 +1361,13 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="9"/>
@@ -1419,13 +1375,13 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -1433,10 +1389,10 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1445,10 +1401,10 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1457,32 +1413,32 @@
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1">
       <c r="A31" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1">
       <c r="A32" s="9" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
@@ -1497,39 +1453,43 @@
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1">
       <c r="A34" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" s="11"/>
+        <v>13</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="C34" s="9" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="9"/>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1">
       <c r="A35" s="9" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="9"/>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1">
       <c r="A36" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="B36" s="9"/>
+        <v>61</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="11"/>
@@ -1537,150 +1497,98 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E37" s="11"/>
       <c r="F37" s="9"/>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1">
       <c r="A38" s="9" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E38" s="11"/>
       <c r="F38" s="9"/>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="B39" s="9"/>
+        <v>83</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="11"/>
       <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="11"/>
       <c r="F40" s="9"/>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1">
-      <c r="A41" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>33</v>
-      </c>
       <c r="D41" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="9"/>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1">
-      <c r="A42" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="15" t="s">
-        <v>35</v>
-      </c>
       <c r="D42" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="9"/>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1">
-      <c r="A43" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="D43" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="9"/>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1">
-      <c r="A44" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="D44" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E44" s="9"/>
       <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1">
-      <c r="A45" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="D45" s="9" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E45" s="9"/>
       <c r="F45" s="9"/>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1">
-      <c r="A46" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="14" t="s">
-        <v>70</v>
-      </c>
       <c r="D46" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E46" s="9"/>
       <c r="F46" s="9"/>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="D47" s="11" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E47" s="9"/>
       <c r="F47" s="9"/>
@@ -1738,451 +1646,451 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="6" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="6" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="6" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="6" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="6" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="6" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="6" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="6" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="6" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="6" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1">
       <c r="A17" s="6" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1">
       <c r="A18" s="6" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1">
       <c r="A19" s="6" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1">
       <c r="A20" s="6" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1">
       <c r="A21" s="6" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
       <c r="A22" s="6" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1">
       <c r="A23" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1">
       <c r="A24" s="6" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1">
       <c r="A25" s="6" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="A26" s="6" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="A27" s="6" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2212,16 +2120,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -2244,562 +2152,562 @@
     </row>
     <row r="4" spans="1:6" ht="30.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="30.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="30.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1">
       <c r="A37" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1">
       <c r="A40" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1">
       <c r="A41" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1">
@@ -2823,4 +2731,99 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" ht="120">
+      <c r="A3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed typos in the excel sheet
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -375,9 +375,6 @@
     <t>We will take you through an introduction of probability and learn concepts such as Bayes rule and conditional probability.  {Press Continue}</t>
   </si>
   <si>
-    <t xml:space="preserve"> So lets begin!  {Press Continue}</t>
-  </si>
-  <si>
     <t>We will first start with the basics of Set Theory. A set is a collection of distinct events or obejcts.  {Press Continue}</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>The law of total probability states that the total probability of all events in a set is 1.  {Press Continue}</t>
   </si>
   <si>
-    <t xml:space="preserve"> Now lets learn about our neuron.  {Press Continue}</t>
-  </si>
-  <si>
     <t>Our neuron is composed of dendrites (D), axons (A), and a axon hillock (AH).  {Press Continue}</t>
   </si>
   <si>
@@ -448,6 +442,12 @@
   </si>
   <si>
     <t>Great Job! That Concludes this lesson. You may go on to the Medium level by typing ready.</t>
+  </si>
+  <si>
+    <t>So lets begin!  {Press Continue}</t>
+  </si>
+  <si>
+    <t>Now lets learn about our neuron.  {Press Continue}</t>
   </si>
 </sst>
 </file>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>39</v>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>39</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>39</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>39</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>39</v>
@@ -1192,7 +1192,7 @@
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>39</v>
@@ -1208,7 +1208,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>39</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>39</v>
@@ -1256,7 +1256,7 @@
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="9" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>39</v>
@@ -1272,7 +1272,7 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>39</v>
@@ -1288,7 +1288,7 @@
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>39</v>
@@ -1328,7 +1328,7 @@
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1">
       <c r="A22" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>39</v>
@@ -1368,7 +1368,7 @@
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B25" s="10" t="s">
         <v>39</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>39</v>
@@ -1400,7 +1400,7 @@
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B27" s="10" t="s">
         <v>39</v>
@@ -1416,7 +1416,7 @@
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>39</v>
@@ -1432,7 +1432,7 @@
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1">
       <c r="A29" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>39</v>
@@ -1448,7 +1448,7 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1">
       <c r="A30" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>39</v>
@@ -1467,7 +1467,7 @@
         <v>41</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>9</v>
@@ -1483,7 +1483,7 @@
         <v>42</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>10</v>
@@ -1507,7 +1507,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>12</v>
@@ -1552,7 +1552,7 @@
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1">
       <c r="A37" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>39</v>
@@ -1584,10 +1584,10 @@
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1">
       <c r="A39" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>36</v>
@@ -2129,7 +2129,7 @@
         <v>109</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>36</v>
@@ -2790,7 +2790,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>

<commit_message>
hard done and gameover
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="164">
   <si>
     <t>question</t>
   </si>
@@ -508,9 +508,6 @@
     <t>Where do you guess the neuron might be? {Press Enter below before clicking a square}</t>
   </si>
   <si>
-    <t xml:space="preserve">If they find part of the neuron they have 8 more chances to locate the rest of the neuron. </t>
-  </si>
-  <si>
     <t>The player has 8 chances to find part of the neuron.  A wise strategy is to start with locations where the axon hillock could reside.</t>
   </si>
   <si>
@@ -524,6 +521,15 @@
   </si>
   <si>
     <t>What was the probability that the axon hillock was there?</t>
+  </si>
+  <si>
+    <t>Tallying score... Press Continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @GameOver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If they find part of the neuron they have more chances to locate the rest of the neuron. </t>
   </si>
 </sst>
 </file>
@@ -2205,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2297,7 +2303,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>4</v>
@@ -2313,7 +2319,7 @@
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>4</v>
@@ -2329,7 +2335,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>4</v>
@@ -2345,7 +2351,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>4</v>
@@ -2361,7 +2367,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="17"/>
@@ -2403,7 +2409,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>79</v>
@@ -2435,7 +2441,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>79</v>
@@ -2467,7 +2473,7 @@
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>79</v>
@@ -2499,7 +2505,7 @@
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>79</v>
@@ -2531,7 +2537,7 @@
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>79</v>
@@ -2563,7 +2569,7 @@
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>79</v>
@@ -2591,7 +2597,7 @@
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>79</v>
@@ -2619,7 +2625,7 @@
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>79</v>
@@ -2632,10 +2638,18 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
+      <c r="A29" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>

</xml_diff>